<commit_message>
appium server log configured for each test scripts and modified excel utility
</commit_message>
<xml_diff>
--- a/src/test/TestData/languages.xlsx
+++ b/src/test/TestData/languages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="hindi" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Teacher and student registration were implemented in base class
</commit_message>
<xml_diff>
--- a/src/test/TestData/languages.xlsx
+++ b/src/test/TestData/languages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hindi" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>माइक ऑन</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Video on</t>
+  </si>
+  <si>
+    <t>Video off</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -494,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -551,7 +554,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>